<commit_message>
cración casos de uso, casos de uso ectendido y diagrama ER
</commit_message>
<xml_diff>
--- a/documentación/REQUERIMIENTOS FRUNACOL.xlsx
+++ b/documentación/REQUERIMIENTOS FRUNACOL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP LAPTOP\Documents\Copia seguridad pc-smart\Copia de seguridad windows\archivos importantes\trabajos sena\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP LAPTOP\Documents\Copia seguridad pc-smart\Copia de seguridad windows\archivos importantes\trabajos sena\Proyecto Frunacol\documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EFE1005-030F-498A-A510-CDE0E76D1053}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E75C5B2-7363-4A13-B251-B28439B48CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{489299F4-CE56-4183-8077-4F7D52D8A63D}"/>
   </bookViews>
@@ -23,6 +23,8 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
   <si>
     <t>FECHA</t>
   </si>
@@ -153,6 +155,12 @@
   </si>
   <si>
     <t>DESCRIPCION ARTICULOS</t>
+  </si>
+  <si>
+    <t>PRODUCTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRESNETACIÓN </t>
   </si>
 </sst>
 </file>
@@ -205,11 +213,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069BF356-7BC2-45DC-8A93-6AA48B62E502}">
-  <dimension ref="A1:Y49"/>
+  <dimension ref="A1:Y67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,32 +550,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="O1" s="1" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="O1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -664,578 +672,578 @@
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>44488</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>123</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>696</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>804</v>
       </c>
-      <c r="F4" s="3">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
         <v>4080</v>
       </c>
-      <c r="H4" s="3">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3">
-        <v>0</v>
-      </c>
-      <c r="M4" s="3">
-        <v>0</v>
-      </c>
-      <c r="O4" s="3">
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
         <v>54</v>
       </c>
-      <c r="P4" s="3">
+      <c r="P4" s="2">
         <v>500</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="Q4" s="2">
         <v>500</v>
       </c>
-      <c r="R4" s="3">
-        <v>0</v>
-      </c>
-      <c r="S4" s="3">
+      <c r="R4" s="2">
+        <v>0</v>
+      </c>
+      <c r="S4" s="2">
         <v>2000</v>
       </c>
-      <c r="T4" s="3">
-        <v>0</v>
-      </c>
-      <c r="U4" s="3">
-        <v>0</v>
-      </c>
-      <c r="V4" s="3">
-        <v>0</v>
-      </c>
-      <c r="W4" s="3">
-        <v>0</v>
-      </c>
-      <c r="X4" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="3">
+      <c r="T4" s="2">
+        <v>0</v>
+      </c>
+      <c r="U4" s="2">
+        <v>0</v>
+      </c>
+      <c r="V4" s="2">
+        <v>0</v>
+      </c>
+      <c r="W4" s="2">
+        <v>0</v>
+      </c>
+      <c r="X4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>500</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2">
         <v>80</v>
       </c>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
-      <c r="V12" s="3"/>
-      <c r="W12" s="3"/>
-      <c r="X12" s="3"/>
-      <c r="Y12" s="3"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="3"/>
-      <c r="W13" s="3"/>
-      <c r="X13" s="3"/>
-      <c r="Y13" s="3"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="3"/>
-      <c r="W14" s="3"/>
-      <c r="X14" s="3"/>
-      <c r="Y14" s="3"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
-      <c r="V15" s="3"/>
-      <c r="W15" s="3"/>
-      <c r="X15" s="3"/>
-      <c r="Y15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
-      <c r="X16" s="3"/>
-      <c r="Y16" s="3"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
-      <c r="V17" s="3"/>
-      <c r="W17" s="3"/>
-      <c r="X17" s="3"/>
-      <c r="Y17" s="3"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-      <c r="Y18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="3"/>
-      <c r="W19" s="3"/>
-      <c r="X19" s="3"/>
-      <c r="Y19" s="3"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
-      <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
-      <c r="V21" s="3"/>
-      <c r="W21" s="3"/>
-      <c r="X21" s="3"/>
-      <c r="Y21" s="3"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
-      <c r="V22" s="3"/>
-      <c r="W22" s="3"/>
-      <c r="X22" s="3"/>
-      <c r="Y22" s="3"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="2"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
-      <c r="V23" s="3"/>
-      <c r="W23" s="3"/>
-      <c r="X23" s="3"/>
-      <c r="Y23" s="3"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D24">
@@ -1251,7 +1259,7 @@
         <v>0</v>
       </c>
       <c r="G24">
-        <f t="shared" si="0"/>
+        <f>SUM(G4:G23)</f>
         <v>4080</v>
       </c>
       <c r="H24">
@@ -1351,7 +1359,7 @@
         <v>0</v>
       </c>
       <c r="G26">
-        <f t="shared" si="1"/>
+        <f>+G24-S24</f>
         <v>2080</v>
       </c>
       <c r="H26">
@@ -1482,6 +1490,61 @@
       </c>
       <c r="G49" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>35</v>
+      </c>
+      <c r="B59" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>35</v>
+      </c>
+      <c r="B63" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>35</v>
+      </c>
+      <c r="B67" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aplicando principios de normalización 1FN,2FN,3FN
</commit_message>
<xml_diff>
--- a/documentación/REQUERIMIENTOS FRUNACOL.xlsx
+++ b/documentación/REQUERIMIENTOS FRUNACOL.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP LAPTOP\Documents\Copia seguridad pc-smart\Copia de seguridad windows\archivos importantes\trabajos sena\Proyecto Frunacol\documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E75C5B2-7363-4A13-B251-B28439B48CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6535AD56-CCAF-45B8-B6AE-5BAABADD2098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{489299F4-CE56-4183-8077-4F7D52D8A63D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -534,19 +535,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069BF356-7BC2-45DC-8A93-6AA48B62E502}">
   <dimension ref="A1:Y67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1"/>
     <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.85546875" customWidth="1"/>
+    <col min="25" max="25" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -587,27 +593,41 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L2" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="M2" s="3"/>
       <c r="O2" t="s">
         <v>1</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="S2" t="s">
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="X2" t="s">
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="Y2" s="3"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
@@ -1548,10 +1568,28 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="8">
     <mergeCell ref="C1:M1"/>
     <mergeCell ref="O1:Y1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="S2:W2"/>
+    <mergeCell ref="P2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39AC412E-703C-4DE4-B298-FA126930E404}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>